<commit_message>
Add Readme | npm start script
</commit_message>
<xml_diff>
--- a/Debt.xlsx
+++ b/Debt.xlsx
@@ -6,21 +6,21 @@
   </bookViews>
   <sheets>
     <sheet name="Liquid Fund" sheetId="1" r:id="rId1"/>
-    <sheet name="Dynamic Fund" sheetId="2" r:id="rId2"/>
-    <sheet name="Corporate Fund" sheetId="3" r:id="rId3"/>
-    <sheet name="Other Fund" sheetId="4" r:id="rId4"/>
+    <sheet name="Dynamic Bond" sheetId="2" r:id="rId2"/>
+    <sheet name="Corporate Bond Fund" sheetId="3" r:id="rId3"/>
+    <sheet name="Other Bond" sheetId="4" r:id="rId4"/>
     <sheet name="Money Market Fund" sheetId="5" r:id="rId5"/>
     <sheet name="Gilt Fund" sheetId="6" r:id="rId6"/>
-    <sheet name="Bank PSU" sheetId="7" r:id="rId7"/>
+    <sheet name="Banking and PSU Fund" sheetId="7" r:id="rId7"/>
     <sheet name="Floater Fund" sheetId="8" r:id="rId8"/>
     <sheet name="Long Duration Fund" sheetId="9" r:id="rId9"/>
     <sheet name="Short Duration Fund" sheetId="10" r:id="rId10"/>
     <sheet name="Medium Duration Fund" sheetId="11" r:id="rId11"/>
     <sheet name="Low Duration Fund" sheetId="12" r:id="rId12"/>
-    <sheet name="Ultra Short Duration" sheetId="13" r:id="rId13"/>
+    <sheet name="Ultra Short Duration Fund" sheetId="13" r:id="rId13"/>
     <sheet name="Credit Risk Fund" sheetId="14" r:id="rId14"/>
-    <sheet name="Medium to Long Duration" sheetId="15" r:id="rId15"/>
-    <sheet name="Gilt 10Y Fund" sheetId="16" r:id="rId16"/>
+    <sheet name="Medium to Long Duration Fund" sheetId="15" r:id="rId15"/>
+    <sheet name="Gilt Fund with 10 year constant duration" sheetId="16" r:id="rId16"/>
     <sheet name="Overnight Fund" sheetId="17" r:id="rId17"/>
   </sheets>
 </workbook>
@@ -1674,13 +1674,13 @@
         <v>0.05</v>
       </c>
       <c r="G4" s="13" t="n">
-        <v>4.6</v>
+        <v>4.59</v>
       </c>
       <c r="H4" s="20" t="n">
-        <v>6.38</v>
+        <v>6.37</v>
       </c>
       <c r="I4" s="20" t="n">
-        <v>6.75</v>
+        <v>6.74</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>13</v>
@@ -1718,7 +1718,7 @@
         <v>4.55</v>
       </c>
       <c r="H5" s="20" t="n">
-        <v>6.26</v>
+        <v>6.25</v>
       </c>
       <c r="I5" s="20" t="n">
         <v>6.65</v>
@@ -1876,16 +1876,16 @@
         <v>0.25</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="G9" s="13" t="n">
         <v>4.34</v>
       </c>
       <c r="H9" s="20" t="n">
-        <v>6.13</v>
+        <v>6.12</v>
       </c>
       <c r="I9" s="20" t="n">
-        <v>6.57</v>
+        <v>6.56</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>13</v>
@@ -1999,16 +1999,16 @@
         <v>0.23</v>
       </c>
       <c r="F12" s="11" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="G12" s="13" t="n">
         <v>4.36</v>
       </c>
       <c r="H12" s="20" t="n">
-        <v>6.14</v>
+        <v>6.13</v>
       </c>
       <c r="I12" s="20" t="n">
-        <v>6.57</v>
+        <v>6.56</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>13</v>
@@ -2128,10 +2128,10 @@
         <v>4.24</v>
       </c>
       <c r="H15" s="20" t="n">
-        <v>6.05</v>
+        <v>6.04</v>
       </c>
       <c r="I15" s="20" t="n">
-        <v>6.52</v>
+        <v>6.51</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>13</v>
@@ -2169,7 +2169,7 @@
         <v>4.41</v>
       </c>
       <c r="H16" s="20" t="n">
-        <v>6.17</v>
+        <v>6.16</v>
       </c>
       <c r="I16" s="20" t="n">
         <v>6.57</v>
@@ -2210,7 +2210,7 @@
         <v>4.51</v>
       </c>
       <c r="H17" s="20" t="n">
-        <v>6.31</v>
+        <v>6.3</v>
       </c>
       <c r="I17" s="20" t="n">
         <v>6.7</v>
@@ -2248,13 +2248,13 @@
         <v>0.04</v>
       </c>
       <c r="G18" s="13" t="n">
-        <v>4.31</v>
+        <v>4.3</v>
       </c>
       <c r="H18" s="20" t="n">
-        <v>6.14</v>
+        <v>6.13</v>
       </c>
       <c r="I18" s="20" t="n">
-        <v>6.6</v>
+        <v>6.59</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>13</v>
@@ -2336,7 +2336,7 @@
         <v>6.3</v>
       </c>
       <c r="I20" s="20" t="n">
-        <v>6.7</v>
+        <v>6.69</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>13</v>
@@ -2368,13 +2368,13 @@
         <v>0.23</v>
       </c>
       <c r="F21" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G21" s="13" t="n">
-        <v>4.4</v>
+        <v>4.39</v>
       </c>
       <c r="H21" s="20" t="n">
-        <v>6.27</v>
+        <v>6.26</v>
       </c>
       <c r="I21" s="20" t="n">
         <v>6.64</v>
@@ -2412,10 +2412,10 @@
         <v>0.04</v>
       </c>
       <c r="G22" s="13" t="n">
-        <v>4.59</v>
+        <v>4.58</v>
       </c>
       <c r="H22" s="20" t="n">
-        <v>6.28</v>
+        <v>6.27</v>
       </c>
       <c r="I22" s="20" t="n">
         <v>6.67</v>
@@ -2450,28 +2450,28 @@
         <v>0.23</v>
       </c>
       <c r="F23" s="11" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="G23" s="13" t="n">
         <v>4.27</v>
       </c>
       <c r="H23" s="20" t="n">
-        <v>6.2</v>
+        <v>6.19</v>
       </c>
       <c r="I23" s="20" t="n">
-        <v>6.61</v>
+        <v>6.6</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="18" t="n">
-        <v>56.88</v>
-      </c>
-      <c r="L23" s="18" t="n">
-        <v>46.77</v>
+      <c r="K23" s="25" t="n">
+        <v>38.54</v>
+      </c>
+      <c r="L23" s="28" t="n">
+        <v>35.1</v>
       </c>
       <c r="M23" s="21" t="n">
-        <v>6.18</v>
+        <v>5.21</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2532,16 +2532,16 @@
         <v>0.18</v>
       </c>
       <c r="F25" s="11" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="G25" s="12" t="n">
-        <v>3.63</v>
+        <v>3.62</v>
       </c>
       <c r="H25" s="16" t="n">
-        <v>5.53</v>
+        <v>5.52</v>
       </c>
       <c r="I25" s="20" t="n">
-        <v>6.03</v>
+        <v>6.02</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>13</v>
@@ -2661,10 +2661,10 @@
         <v>4.53</v>
       </c>
       <c r="H28" s="20" t="n">
-        <v>6.32</v>
+        <v>6.31</v>
       </c>
       <c r="I28" s="20" t="n">
-        <v>6.53</v>
+        <v>6.52</v>
       </c>
       <c r="J28" s="8" t="s">
         <v>13</v>
@@ -2713,11 +2713,11 @@
       <c r="K29" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L29" s="29" t="n">
-        <v>31.54</v>
+      <c r="L29" s="19" t="n">
+        <v>10.91</v>
       </c>
       <c r="M29" s="18" t="n">
-        <v>63.51</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2781,13 +2781,13 @@
         <v>0.04</v>
       </c>
       <c r="G31" s="13" t="n">
-        <v>4.58</v>
+        <v>4.57</v>
       </c>
       <c r="H31" s="20" t="n">
-        <v>6.26</v>
+        <v>6.25</v>
       </c>
       <c r="I31" s="20" t="n">
-        <v>6.68</v>
+        <v>6.67</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>13</v>
@@ -2819,16 +2819,16 @@
         <v>0.21</v>
       </c>
       <c r="F32" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G32" s="13" t="n">
         <v>4.43</v>
       </c>
       <c r="H32" s="20" t="n">
-        <v>6.21</v>
+        <v>6.2</v>
       </c>
       <c r="I32" s="20" t="n">
-        <v>6.55</v>
+        <v>6.54</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>13</v>
@@ -2860,16 +2860,16 @@
         <v>0.13</v>
       </c>
       <c r="F33" s="11" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="G33" s="13" t="n">
         <v>4.43</v>
       </c>
       <c r="H33" s="20" t="n">
-        <v>6.24</v>
+        <v>6.23</v>
       </c>
       <c r="I33" s="20" t="n">
-        <v>6.64</v>
+        <v>6.63</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>13</v>
@@ -2907,10 +2907,10 @@
         <v>4.5</v>
       </c>
       <c r="H34" s="20" t="n">
-        <v>6.27</v>
+        <v>6.26</v>
       </c>
       <c r="I34" s="20" t="n">
-        <v>6.68</v>
+        <v>6.67</v>
       </c>
       <c r="J34" s="8" t="s">
         <v>13</v>
@@ -2948,7 +2948,7 @@
         <v>4.41</v>
       </c>
       <c r="H35" s="20" t="n">
-        <v>6.22</v>
+        <v>6.21</v>
       </c>
       <c r="I35" s="20" t="n">
         <v>6.63</v>
@@ -2989,7 +2989,7 @@
         <v>4.42</v>
       </c>
       <c r="H36" s="20" t="n">
-        <v>6.19</v>
+        <v>6.18</v>
       </c>
       <c r="I36" s="20" t="n">
         <v>6.62</v>
@@ -3024,16 +3024,16 @@
         <v>0.25</v>
       </c>
       <c r="F37" s="11" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="G37" s="13" t="n">
-        <v>4.4</v>
+        <v>4.39</v>
       </c>
       <c r="H37" s="20" t="n">
-        <v>6.26</v>
+        <v>6.25</v>
       </c>
       <c r="I37" s="20" t="n">
-        <v>6.71</v>
+        <v>6.7</v>
       </c>
       <c r="J37" s="8" t="s">
         <v>13</v>
@@ -3065,16 +3065,16 @@
         <v>0.22</v>
       </c>
       <c r="F38" s="11" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="G38" s="12" t="n">
-        <v>3.85</v>
+        <v>3.84</v>
       </c>
       <c r="H38" s="16" t="n">
-        <v>5.94</v>
+        <v>5.93</v>
       </c>
       <c r="I38" s="20" t="n">
-        <v>6.54</v>
+        <v>6.53</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>13</v>
@@ -3147,13 +3147,13 @@
         <v>0.19</v>
       </c>
       <c r="F40" s="11" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="G40" s="12" t="n">
-        <v>3.8</v>
+        <v>3.79</v>
       </c>
       <c r="H40" s="16" t="n">
-        <v>5.84</v>
+        <v>5.83</v>
       </c>
       <c r="I40" s="11" t="n">
         <v>0</v>
@@ -3229,7 +3229,7 @@
         <v>0.14</v>
       </c>
       <c r="F42" s="11" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="G42" s="12" t="n">
         <v>3.86</v>
@@ -3273,7 +3273,7 @@
         <v>0.05</v>
       </c>
       <c r="G43" s="12" t="n">
-        <v>3.45</v>
+        <v>3.44</v>
       </c>
       <c r="H43" s="11" t="n">
         <v>0</v>
@@ -3311,10 +3311,10 @@
         <v>0.31</v>
       </c>
       <c r="F44" s="11" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="G44" s="16" t="n">
-        <v>5.43</v>
+        <v>5.42</v>
       </c>
       <c r="H44" s="20" t="n">
         <v>6.76</v>
@@ -4354,14 +4354,14 @@
       <c r="J16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="36" t="n">
-        <v>17.48</v>
+      <c r="K16" s="22" t="n">
+        <v>23.06</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M16" s="18" t="n">
-        <v>53.86</v>
+        <v>66.86</v>
       </c>
       <c r="N16" s="8" t="s">
         <v>13</v>
@@ -4373,7 +4373,7 @@
         <v>13</v>
       </c>
       <c r="Q16" s="21" t="n">
-        <v>4.12</v>
+        <v>4.11</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>13</v>
@@ -4549,14 +4549,14 @@
       <c r="J19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="22" t="n">
-        <v>24.45</v>
+      <c r="K19" s="28" t="n">
+        <v>34.5</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M19" s="18" t="n">
-        <v>70</v>
+        <v>59.24</v>
       </c>
       <c r="N19" s="8" t="s">
         <v>13</v>
@@ -7738,14 +7738,14 @@
       <c r="J18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="19" t="n">
-        <v>11.12</v>
-      </c>
-      <c r="L18" s="27" t="n">
-        <v>21.89</v>
+      <c r="K18" s="36" t="n">
+        <v>13.47</v>
+      </c>
+      <c r="L18" s="36" t="n">
+        <v>16.75</v>
       </c>
       <c r="M18" s="18" t="n">
-        <v>61.79</v>
+        <v>60.18</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>13</v>
@@ -7942,14 +7942,14 @@
       <c r="J21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="36" t="n">
-        <v>14.33</v>
-      </c>
-      <c r="L21" s="29" t="n">
-        <v>31.3</v>
-      </c>
-      <c r="M21" s="18" t="n">
-        <v>51.15</v>
+      <c r="K21" s="29" t="n">
+        <v>30.32</v>
+      </c>
+      <c r="L21" s="21" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="M21" s="28" t="n">
+        <v>37.76</v>
       </c>
       <c r="N21" s="8" t="s">
         <v>13</v>
@@ -9655,14 +9655,14 @@
       <c r="J18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="24" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="L18" s="27" t="n">
-        <v>18.68</v>
-      </c>
-      <c r="M18" s="18" t="n">
-        <v>75.9</v>
+      <c r="K18" s="18" t="n">
+        <v>57.63</v>
+      </c>
+      <c r="L18" s="21" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="M18" s="22" t="n">
+        <v>23.72</v>
       </c>
       <c r="N18" s="8" t="s">
         <v>13</v>
@@ -10539,14 +10539,14 @@
       <c r="J31" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="27" t="n">
-        <v>21.9</v>
+      <c r="K31" s="29" t="n">
+        <v>30.87</v>
       </c>
       <c r="L31" s="18" t="n">
-        <v>56.78</v>
-      </c>
-      <c r="M31" s="27" t="n">
-        <v>20.56</v>
+        <v>47.15</v>
+      </c>
+      <c r="M31" s="36" t="n">
+        <v>17</v>
       </c>
       <c r="N31" s="8" t="s">
         <v>13</v>
@@ -13187,13 +13187,13 @@
         <v>13</v>
       </c>
       <c r="K13" s="18" t="n">
-        <v>76.25</v>
+        <v>85.79</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M13" s="19" t="n">
-        <v>8.56</v>
+      <c r="M13" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>13</v>
@@ -13258,13 +13258,13 @@
         <v>13</v>
       </c>
       <c r="K14" s="18" t="n">
-        <v>62.35</v>
+        <v>62.54</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="28" t="n">
-        <v>33.53</v>
+      <c r="M14" s="29" t="n">
+        <v>32.93</v>
       </c>
       <c r="N14" s="8" t="s">
         <v>13</v>
@@ -14050,16 +14050,16 @@
         <v>0.17</v>
       </c>
       <c r="F2" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G2" s="12" t="n">
-        <v>3.47</v>
+        <v>3.46</v>
       </c>
       <c r="H2" s="16" t="n">
         <v>5.13</v>
       </c>
       <c r="I2" s="16" t="n">
-        <v>5.58</v>
+        <v>5.57</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>13</v>
@@ -14124,13 +14124,13 @@
         <v>0.05</v>
       </c>
       <c r="G3" s="12" t="n">
-        <v>3.51</v>
+        <v>3.49</v>
       </c>
       <c r="H3" s="16" t="n">
-        <v>5.17</v>
+        <v>5.16</v>
       </c>
       <c r="I3" s="16" t="n">
-        <v>5.68</v>
+        <v>5.67</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>13</v>
@@ -14192,13 +14192,13 @@
         <v>0.72</v>
       </c>
       <c r="F4" s="11" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="G4" s="12" t="n">
-        <v>3.56</v>
+        <v>3.55</v>
       </c>
       <c r="H4" s="13" t="n">
-        <v>4.99</v>
+        <v>4.95</v>
       </c>
       <c r="I4" s="16" t="n">
         <v>5.89</v>
@@ -14266,10 +14266,10 @@
         <v>0.05</v>
       </c>
       <c r="G5" s="12" t="n">
-        <v>3.54</v>
+        <v>3.53</v>
       </c>
       <c r="H5" s="16" t="n">
-        <v>5.23</v>
+        <v>5.22</v>
       </c>
       <c r="I5" s="16" t="n">
         <v>5.87</v>
@@ -14334,10 +14334,10 @@
         <v>0.12</v>
       </c>
       <c r="F6" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G6" s="12" t="n">
-        <v>3.49</v>
+        <v>3.48</v>
       </c>
       <c r="H6" s="11" t="n">
         <v>0</v>
@@ -14405,10 +14405,10 @@
         <v>0.12</v>
       </c>
       <c r="F7" s="11" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="G7" s="12" t="n">
-        <v>3.58</v>
+        <v>3.57</v>
       </c>
       <c r="H7" s="11" t="n">
         <v>0</v>
@@ -14479,7 +14479,7 @@
         <v>0.05</v>
       </c>
       <c r="G8" s="12" t="n">
-        <v>3.52</v>
+        <v>3.51</v>
       </c>
       <c r="H8" s="11" t="n">
         <v>0</v>
@@ -14547,10 +14547,10 @@
         <v>0.12</v>
       </c>
       <c r="F9" s="11" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="G9" s="12" t="n">
-        <v>3.69</v>
+        <v>3.67</v>
       </c>
       <c r="H9" s="11" t="n">
         <v>0</v>
@@ -14618,10 +14618,10 @@
         <v>0.12</v>
       </c>
       <c r="F10" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G10" s="12" t="n">
-        <v>3.5</v>
+        <v>3.49</v>
       </c>
       <c r="H10" s="11" t="n">
         <v>0</v>
@@ -14692,7 +14692,7 @@
         <v>0.05</v>
       </c>
       <c r="G11" s="12" t="n">
-        <v>3.5</v>
+        <v>3.49</v>
       </c>
       <c r="H11" s="11" t="n">
         <v>0</v>
@@ -14760,10 +14760,10 @@
         <v>0.07</v>
       </c>
       <c r="F12" s="11" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="G12" s="12" t="n">
-        <v>3.55</v>
+        <v>3.54</v>
       </c>
       <c r="H12" s="11" t="n">
         <v>0</v>
@@ -14834,7 +14834,7 @@
         <v>0.05</v>
       </c>
       <c r="G13" s="12" t="n">
-        <v>3.56</v>
+        <v>3.55</v>
       </c>
       <c r="H13" s="11" t="n">
         <v>0</v>
@@ -14902,10 +14902,10 @@
         <v>0.09</v>
       </c>
       <c r="F14" s="11" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="G14" s="12" t="n">
-        <v>3.53</v>
+        <v>3.52</v>
       </c>
       <c r="H14" s="11" t="n">
         <v>0</v>
@@ -15044,10 +15044,10 @@
         <v>0.11</v>
       </c>
       <c r="F16" s="11" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="G16" s="12" t="n">
-        <v>3.58</v>
+        <v>3.56</v>
       </c>
       <c r="H16" s="11" t="n">
         <v>0</v>
@@ -15118,7 +15118,7 @@
         <v>0.06</v>
       </c>
       <c r="G17" s="12" t="n">
-        <v>3.59</v>
+        <v>3.58</v>
       </c>
       <c r="H17" s="11" t="n">
         <v>0</v>
@@ -15186,10 +15186,10 @@
         <v>0.1</v>
       </c>
       <c r="F18" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G18" s="12" t="n">
-        <v>3.39</v>
+        <v>3.38</v>
       </c>
       <c r="H18" s="11" t="n">
         <v>0</v>
@@ -15257,10 +15257,10 @@
         <v>0.1</v>
       </c>
       <c r="F19" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G19" s="12" t="n">
-        <v>3.58</v>
+        <v>3.57</v>
       </c>
       <c r="H19" s="11" t="n">
         <v>0</v>
@@ -15402,7 +15402,7 @@
         <v>0.05</v>
       </c>
       <c r="G21" s="12" t="n">
-        <v>3.54</v>
+        <v>3.53</v>
       </c>
       <c r="H21" s="11" t="n">
         <v>0</v>
@@ -15615,7 +15615,7 @@
         <v>0.06</v>
       </c>
       <c r="G24" s="12" t="n">
-        <v>3.7</v>
+        <v>3.69</v>
       </c>
       <c r="H24" s="11" t="n">
         <v>0</v>
@@ -15683,10 +15683,10 @@
         <v>0.1</v>
       </c>
       <c r="F25" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G25" s="12" t="n">
-        <v>3.39</v>
+        <v>3.38</v>
       </c>
       <c r="H25" s="11" t="n">
         <v>0</v>
@@ -15757,7 +15757,7 @@
         <v>0.05</v>
       </c>
       <c r="G26" s="12" t="n">
-        <v>3.47</v>
+        <v>3.46</v>
       </c>
       <c r="H26" s="11" t="n">
         <v>0</v>
@@ -15825,10 +15825,10 @@
         <v>0.09</v>
       </c>
       <c r="F27" s="11" t="n">
-        <v>0.05</v>
+        <v>0.07</v>
       </c>
       <c r="G27" s="12" t="n">
-        <v>3.68</v>
+        <v>3.67</v>
       </c>
       <c r="H27" s="11" t="n">
         <v>0</v>
@@ -15899,7 +15899,7 @@
         <v>0.06</v>
       </c>
       <c r="G28" s="12" t="n">
-        <v>3.74</v>
+        <v>3.73</v>
       </c>
       <c r="H28" s="11" t="n">
         <v>0</v>
@@ -17048,13 +17048,13 @@
         <v>13</v>
       </c>
       <c r="K16" s="18" t="n">
-        <v>80.34</v>
+        <v>77.77</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M16" s="19" t="n">
-        <v>7.7</v>
+        <v>7.86</v>
       </c>
       <c r="N16" s="8" t="s">
         <v>13</v>
@@ -17440,13 +17440,13 @@
         <v>13</v>
       </c>
       <c r="K23" s="18" t="n">
-        <v>86.71</v>
+        <v>90.27</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M23" s="21" t="n">
-        <v>3.64</v>
+        <v>4.42</v>
       </c>
       <c r="N23" s="8" t="s">
         <v>13</v>
@@ -18838,14 +18838,14 @@
       <c r="J15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="27" t="n">
-        <v>20.67</v>
+      <c r="K15" s="29" t="n">
+        <v>29.09</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="M15" s="18" t="n">
-        <v>74.65</v>
+        <v>63.43</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>13</v>
@@ -22594,7 +22594,7 @@
         <v>13</v>
       </c>
       <c r="K20" s="18" t="n">
-        <v>91.92</v>
+        <v>93.32</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>13</v>
@@ -22659,7 +22659,7 @@
         <v>13</v>
       </c>
       <c r="K21" s="18" t="n">
-        <v>91.92</v>
+        <v>93.32</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>13</v>
@@ -22724,7 +22724,7 @@
         <v>13</v>
       </c>
       <c r="K22" s="18" t="n">
-        <v>91.92</v>
+        <v>93.32</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>13</v>

</xml_diff>